<commit_message>
Revert "Merge branch 'master' of https://github.com/Ymiku/PaymentAppSimulator"
This reverts commit 6ef35a3a9d32f993b2a259609b34c139e7745f43, reversing
changes made to a176bb7bbac6242a6f80a5ee1a8d04604ea537f6.
</commit_message>
<xml_diff>
--- a/DataConfig/Excel/content.xlsx
+++ b/DataConfig/Excel/content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\PaymentAppSimulator\DataConfig\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5699AD-1353-44F7-B845-8A26A3FAC3BA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764F3B4B-1FB5-4C1D-B98F-1810CA2716DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>required</t>
   </si>
@@ -94,25 +94,6 @@
   <si>
     <t>未设置昵称</t>
     <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>新密码不能与以前密码相同</t>
-  </si>
-  <si>
-    <t>修改支付密码成功</t>
-  </si>
-  <si>
-    <t>两次输入密码不一致</t>
-  </si>
-  <si>
-    <t>支付密码不能是重复、连续的数字</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置支付密码</t>
-  </si>
-  <si>
-    <t>修改支付密码</t>
   </si>
 </sst>
 </file>
@@ -950,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP26"/>
+  <dimension ref="A1:BP20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1192,54 +1173,6 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="4">
-        <v>17</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="4">
-        <v>18</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="4">
-        <v>19</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
-        <v>20</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
-        <v>21</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
-        <v>22</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/Ymiku/PaymentAppSimulator""
This reverts commit 9763b4b95fcef0f2d69533e8c6b49ba58c10d875.
</commit_message>
<xml_diff>
--- a/DataConfig/Excel/content.xlsx
+++ b/DataConfig/Excel/content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\PaymentAppSimulator\DataConfig\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764F3B4B-1FB5-4C1D-B98F-1810CA2716DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5699AD-1353-44F7-B845-8A26A3FAC3BA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>required</t>
   </si>
@@ -94,6 +94,25 @@
   <si>
     <t>未设置昵称</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>新密码不能与以前密码相同</t>
+  </si>
+  <si>
+    <t>修改支付密码成功</t>
+  </si>
+  <si>
+    <t>两次输入密码不一致</t>
+  </si>
+  <si>
+    <t>支付密码不能是重复、连续的数字</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置支付密码</t>
+  </si>
+  <si>
+    <t>修改支付密码</t>
   </si>
 </sst>
 </file>
@@ -931,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP20"/>
+  <dimension ref="A1:BP26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1173,6 +1192,54 @@
         <v>23</v>
       </c>
     </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>17</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>18</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>19</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>20</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>21</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>22</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>